<commit_message>
Fix stile di demo.xlsx e template.xlsx
</commit_message>
<xml_diff>
--- a/demo.xlsx
+++ b/demo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Playground\OM-generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D325F8BB-8DD3-4355-81E2-CD9BF6C9FD98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87D5C8C-D04B-4616-8556-D17CCBF22B90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{A6284BC5-6B1C-4AAC-A778-7781014D47CB}"/>
+    <workbookView xWindow="-28920" yWindow="-2595" windowWidth="29040" windowHeight="15840" xr2:uid="{A6284BC5-6B1C-4AAC-A778-7781014D47CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Dati Input" sheetId="1" r:id="rId1"/>
@@ -359,7 +359,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -374,8 +374,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -387,8 +393,20 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59996337778862885"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -396,14 +414,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutrale" xfId="1" builtinId="28"/>
@@ -721,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE574F61-8D22-4F7C-8066-8994DEC90BEE}">
   <dimension ref="A2:J22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:J22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -731,10 +772,10 @@
     <col min="2" max="2" width="21.33203125" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -772,357 +813,448 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="2">
         <v>1</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J4" t="s">
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="D5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="D7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="D8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="3" t="s">
         <v>38</v>
       </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="3" t="s">
         <v>43</v>
       </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="D10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="3" t="s">
         <v>47</v>
       </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="D11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="J11" t="s">
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="3" t="s">
         <v>55</v>
       </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="D13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="3" t="s">
         <v>59</v>
       </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="D14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="3" t="s">
         <v>59</v>
       </c>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="3" t="s">
         <v>66</v>
       </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="D16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D17" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="D17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="J18" t="s">
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="D19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D21" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="D21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D22" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="D22" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="3" t="s">
         <v>47</v>
       </c>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1133,8 +1265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7043AEE0-0583-4631-9900-7179DD94C0E7}">
   <dimension ref="A2:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:J11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1143,10 +1275,10 @@
     <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1184,167 +1316,204 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="2">
         <v>1</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="J4" t="s">
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="3" t="s">
         <v>90</v>
       </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="D7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="3" t="s">
         <v>47</v>
       </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="D8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="3" t="s">
         <v>47</v>
       </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="D9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="3" t="s">
         <v>47</v>
       </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J10" t="s">
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="D11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="D11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="3" t="s">
         <v>59</v>
       </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix PascalNotation campi complessi
</commit_message>
<xml_diff>
--- a/demo.xlsx
+++ b/demo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Playground\OM-generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87D5C8C-D04B-4616-8556-D17CCBF22B90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40C077A-3678-4A95-A692-6DC5CB63F846}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2595" windowWidth="29040" windowHeight="15840" xr2:uid="{A6284BC5-6B1C-4AAC-A778-7781014D47CB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A6284BC5-6B1C-4AAC-A778-7781014D47CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Dati Input" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="108">
   <si>
     <t>ESEMPIO id rif.</t>
   </si>
@@ -199,9 +199,6 @@
     <t>1.5</t>
   </si>
   <si>
-    <t>serpente</t>
-  </si>
-  <si>
     <t>Diametro</t>
   </si>
   <si>
@@ -353,6 +350,12 @@
   </si>
   <si>
     <t>1.2.1</t>
+  </si>
+  <si>
+    <t>serpente raro</t>
+  </si>
+  <si>
+    <t>personaBella</t>
   </si>
 </sst>
 </file>
@@ -763,7 +766,7 @@
   <dimension ref="A2:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1027,7 +1030,7 @@
         <v>54</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>55</v>
+        <v>106</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -1037,19 +1040,19 @@
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="D13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="3" t="s">
+      <c r="F13" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -1059,19 +1062,19 @@
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="F14" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -1081,19 +1084,19 @@
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E15" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -1103,16 +1106,16 @@
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>47</v>
@@ -1125,19 +1128,19 @@
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="3" t="s">
+      <c r="F17" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -1147,40 +1150,40 @@
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>74</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E18" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="D19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>80</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>47</v>
@@ -1193,19 +1196,19 @@
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>30</v>
+        <v>107</v>
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
@@ -1215,16 +1218,16 @@
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="D21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>86</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>47</v>
@@ -1246,7 +1249,7 @@
         <v>18</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>47</v>
@@ -1338,10 +1341,10 @@
         <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>89</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>14</v>
@@ -1350,7 +1353,7 @@
         <v>19</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -1362,19 +1365,19 @@
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>91</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -1384,16 +1387,16 @@
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>94</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>30</v>
@@ -1406,16 +1409,16 @@
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>47</v>
@@ -1437,7 +1440,7 @@
         <v>18</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>47</v>
@@ -1450,16 +1453,16 @@
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>47</v>
@@ -1472,10 +1475,10 @@
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>102</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>28</v>
@@ -1484,7 +1487,7 @@
         <v>24</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -1496,19 +1499,19 @@
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>106</v>
-      </c>
       <c r="F11" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>

</xml_diff>

<commit_message>
Aggiunta colonna "Caso Test" per aggiungere valore mock personalizzato al campo
</commit_message>
<xml_diff>
--- a/demo.xlsx
+++ b/demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Playground\OM-generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40C077A-3678-4A95-A692-6DC5CB63F846}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E954BFE-D947-4DAD-8EA8-CAD0419FA36D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A6284BC5-6B1C-4AAC-A778-7781014D47CB}"/>
+    <workbookView xWindow="-28920" yWindow="-2595" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A6284BC5-6B1C-4AAC-A778-7781014D47CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Dati Input" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="113">
   <si>
     <t>ESEMPIO id rif.</t>
   </si>
@@ -356,6 +356,21 @@
   </si>
   <si>
     <t>personaBella</t>
+  </si>
+  <si>
+    <t>Caso Test</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>efd</t>
+  </si>
+  <si>
+    <t>ghi</t>
+  </si>
+  <si>
+    <t>jkl</t>
   </si>
 </sst>
 </file>
@@ -763,10 +778,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE574F61-8D22-4F7C-8066-8994DEC90BEE}">
-  <dimension ref="A2:J22"/>
+  <dimension ref="A2:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -783,7 +798,7 @@
     <col min="10" max="10" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -814,8 +829,11 @@
       <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K2" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -832,8 +850,9 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -858,8 +877,11 @@
       <c r="J4" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K4" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
         <v>22</v>
@@ -880,8 +902,11 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K5" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
         <v>26</v>
@@ -902,8 +927,9 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
         <v>31</v>
@@ -924,8 +950,11 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K7" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
         <v>35</v>
@@ -946,8 +975,11 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K8" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
         <v>39</v>
@@ -968,8 +1000,9 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
         <v>44</v>
@@ -990,8 +1023,11 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K10" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
         <v>48</v>
@@ -1014,8 +1050,11 @@
       <c r="J11" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K11" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
         <v>52</v>
@@ -1036,8 +1075,9 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3" t="s">
         <v>55</v>
@@ -1058,8 +1098,11 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K13" s="3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
         <v>59</v>
@@ -1080,8 +1123,11 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K14" s="3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
         <v>62</v>
@@ -1102,8 +1148,9 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
         <v>66</v>
@@ -1124,8 +1171,11 @@
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K16" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
         <v>69</v>
@@ -1146,8 +1196,11 @@
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K17" s="3">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
         <v>72</v>
@@ -1170,8 +1223,9 @@
       <c r="J18" s="3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K18" s="3"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
         <v>77</v>
@@ -1192,8 +1246,11 @@
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K19" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3" t="s">
         <v>80</v>
@@ -1214,8 +1271,9 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K20" s="3"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3" t="s">
         <v>83</v>
@@ -1236,8 +1294,11 @@
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K21" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
         <v>31</v>
@@ -1258,6 +1319,9 @@
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
+      <c r="K22" s="3" t="s">
+        <v>112</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1266,10 +1330,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7043AEE0-0583-4631-9900-7179DD94C0E7}">
-  <dimension ref="A2:J11"/>
+  <dimension ref="A2:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1286,7 +1350,7 @@
     <col min="10" max="10" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1317,8 +1381,11 @@
       <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K2" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1335,8 +1402,9 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -1361,8 +1429,9 @@
       <c r="J4" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
         <v>89</v>
@@ -1383,8 +1452,9 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
         <v>92</v>
@@ -1405,8 +1475,9 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
         <v>95</v>
@@ -1427,8 +1498,11 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K7" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
         <v>36</v>
@@ -1449,8 +1523,11 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K8" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
         <v>84</v>
@@ -1471,8 +1548,11 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K9" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
         <v>100</v>
@@ -1495,8 +1575,11 @@
       <c r="J10" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K10" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
         <v>103</v>
@@ -1517,6 +1600,9 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
+      <c r="K11" s="3">
+        <v>123</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>